<commit_message>
Importar tarjetas terminado (aparentemente)
</commit_message>
<xml_diff>
--- a/arc/arc_Libro4.xlsx
+++ b/arc/arc_Libro4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duvanrivera\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9056D68B-2C68-4DEC-9992-400BB314716C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BB1282-E2EC-4082-890D-DEB3E51BACC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11355" yWindow="1095" windowWidth="18180" windowHeight="11385" xr2:uid="{83EB8D65-2FC0-49AE-950B-5A8B69ED4B02}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="13350" windowHeight="11385" xr2:uid="{83EB8D65-2FC0-49AE-950B-5A8B69ED4B02}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>DUVAN RIVERA</t>
   </si>
@@ -94,9 +94,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -183,13 +180,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016CE917-B376-4331-BB87-E250E38DC066}">
-  <dimension ref="B3:M11"/>
+  <dimension ref="B3:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,49 +521,37 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2">
         <v>1072642921</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1069304404</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>1</v>
+      <c r="E3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1100953829</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="H3" s="10">
-        <v>45317</v>
-      </c>
-      <c r="I3" s="9">
-        <v>1069304404</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1072642921</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" s="10">
-        <v>45438</v>
-      </c>
+        <v>45470</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="10"/>
     </row>
     <row r="4" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D4" s="2">
         <v>1072642921</v>
@@ -574,27 +559,37 @@
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="3">
-        <v>80200165</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="11">
-        <v>45257</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="12"/>
+      <c r="F4" s="4">
+        <v>1069304404</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="10">
+        <v>45444</v>
+      </c>
+      <c r="I4" s="9">
+        <v>1069304404</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1072642921</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="10">
+        <v>45438</v>
+      </c>
     </row>
     <row r="5" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2">
         <v>1072642921</v>
@@ -603,13 +598,13 @@
         <v>4</v>
       </c>
       <c r="F5" s="3">
-        <v>80059515</v>
+        <v>80200165</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H5" s="11">
-        <v>45244</v>
+        <v>45257</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -619,9 +614,11 @@
     </row>
     <row r="6" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="D6" s="2">
         <v>1072642921</v>
       </c>
@@ -629,13 +626,13 @@
         <v>4</v>
       </c>
       <c r="F6" s="3">
-        <v>1076240985</v>
+        <v>80059515</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6" s="11">
-        <v>45454</v>
+        <v>45244</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -645,7 +642,7 @@
     </row>
     <row r="7" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="2">
@@ -655,13 +652,13 @@
         <v>4</v>
       </c>
       <c r="F7" s="3">
-        <v>80370195</v>
+        <v>1076240985</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H7" s="11">
-        <v>45467</v>
+        <v>45454</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -671,7 +668,7 @@
     </row>
     <row r="8" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="2">
@@ -681,94 +678,122 @@
         <v>4</v>
       </c>
       <c r="F8" s="3">
-        <v>1024530115</v>
+        <v>80370195</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H8" s="11">
-        <v>45462</v>
-      </c>
-      <c r="I8" s="8">
-        <v>1024530115</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="2">
-        <v>1072642921</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="M8" s="11">
-        <v>45481</v>
-      </c>
+        <v>45467</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="12"/>
     </row>
     <row r="9" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="2">
+        <v>1072642921</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1024530115</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="11">
+        <v>45462</v>
+      </c>
+      <c r="I9" s="8">
+        <v>1024530115</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1072642921</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="M9" s="11">
+        <v>45481</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="2">
-        <v>1072642921</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="D10" s="2">
+        <v>1072642921</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3">
         <v>1055314236</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H10" s="11">
         <v>45463</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="12"/>
-    </row>
-    <row r="10" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="12"/>
+    </row>
+    <row r="11" spans="2:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="2">
-        <v>1072642921</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="3">
+      <c r="C11" s="5"/>
+      <c r="D11" s="2">
+        <v>1072642921</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="3">
         <v>1100953829</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H11" s="11">
         <v>45146</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I11" s="8">
         <v>1100953829</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="2">
-        <v>1072642921</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="M10" s="12"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
+      <c r="K11" s="2">
+        <v>1072642921</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" s="11">
+        <v>45481</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Base de datos con registros importados
</commit_message>
<xml_diff>
--- a/arc/arc_Libro4.xlsx
+++ b/arc/arc_Libro4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duvanrivera\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474144CE-3B40-4345-9A0C-BB0FDAB5C856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02362E43-24BA-43A9-8658-82E19C13342B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14340" yWindow="1650" windowWidth="13350" windowHeight="11385" xr2:uid="{83EB8D65-2FC0-49AE-950B-5A8B69ED4B02}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>DUVAN RIVERA</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>0001802290 027,32818</t>
+  </si>
+  <si>
+    <t>4545987</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
   <dimension ref="B3:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:M10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +673,9 @@
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="D8" s="2">
         <v>1072642921</v>
       </c>

</xml_diff>